<commit_message>
Update latest data and code
</commit_message>
<xml_diff>
--- a/data/source/weekly/cs-en-us-001pct.xlsx
+++ b/data/source/weekly/cs-en-us-001pct.xlsx
@@ -69,7 +69,7 @@
         <family val="2"/>
         <rFont val="Andale WT"/>
       </rPr>
-      <t xml:space="preserve">38</t>
+      <t xml:space="preserve">40</t>
     </r>
   </si>
   <si>
@@ -95,7 +95,7 @@
         <family val="2"/>
         <rFont val="Andale WT"/>
       </rPr>
-      <t xml:space="preserve">9/19/2022</t>
+      <t xml:space="preserve">10/3/2022</t>
     </r>
     <r>
       <rPr>
@@ -113,7 +113,7 @@
         <family val="2"/>
         <rFont val="Andale WT"/>
       </rPr>
-      <t xml:space="preserve">9/25/2022</t>
+      <t xml:space="preserve">10/9/2022</t>
     </r>
   </si>
   <si>
@@ -866,17 +866,17 @@
       <c r="A15" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C15" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="15">
         <v>1</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" s="15">
-        <v>2</v>
       </c>
       <c r="G15" s="14" t="s">
         <v>20</v>
@@ -894,7 +894,7 @@
         <v>54.545454545454</v>
       </c>
       <c r="L15" s="16">
-        <v>6.25</v>
+        <v>-5.555555555555</v>
       </c>
       <c r="M15" s="16">
         <v>750</v>
@@ -908,13 +908,13 @@
         <v>23</v>
       </c>
       <c r="C16" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" s="15">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E16" s="16">
-        <v>-83.333333333333</v>
+        <v>-50</v>
       </c>
       <c r="F16" s="15">
         <v>8</v>
@@ -926,22 +926,22 @@
         <v>-50</v>
       </c>
       <c r="I16" s="15">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="J16" s="15">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="K16" s="16">
-        <v>15.116279069767</v>
+        <v>14.130434782608</v>
       </c>
       <c r="L16" s="16">
-        <v>-6.603773584905</v>
+        <v>-7.894736842105</v>
       </c>
       <c r="M16" s="16">
-        <v>62.295081967213</v>
+        <v>56.716417910447</v>
       </c>
       <c r="N16" s="16">
-        <v>-84.458398744113</v>
+        <v>-84.162895927601</v>
       </c>
     </row>
     <row r="17" spans="1:14">
@@ -949,40 +949,40 @@
         <v>24</v>
       </c>
       <c r="C17" s="15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D17" s="15">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E17" s="16">
-        <v>100</v>
+        <v>-40</v>
       </c>
       <c r="F17" s="15">
+        <v>7</v>
+      </c>
+      <c r="G17" s="15">
         <v>12</v>
       </c>
-      <c r="G17" s="15">
-        <v>8</v>
-      </c>
       <c r="H17" s="16">
-        <v>50</v>
+        <v>-41.666666666666</v>
       </c>
       <c r="I17" s="15">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="J17" s="15">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="K17" s="16">
-        <v>16.279069767441</v>
+        <v>10.638297872340</v>
       </c>
       <c r="L17" s="16">
-        <v>72.413793103448</v>
+        <v>73.333333333333</v>
       </c>
       <c r="M17" s="16">
-        <v>81.818181818181</v>
+        <v>85.714285714285</v>
       </c>
       <c r="N17" s="16">
-        <v>-27.536231884058</v>
+        <v>-28.275862068965</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -990,40 +990,40 @@
         <v>25</v>
       </c>
       <c r="C18" s="15">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D18" s="15">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E18" s="16">
-        <v>33.333333333333</v>
+        <v>-66.666666666666</v>
       </c>
       <c r="F18" s="15">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G18" s="15">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H18" s="16">
-        <v>-50</v>
+        <v>-29.411764705882</v>
       </c>
       <c r="I18" s="15">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="J18" s="15">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="K18" s="16">
-        <v>70</v>
+        <v>62.184873949579</v>
       </c>
       <c r="L18" s="16">
-        <v>-1.578947368421</v>
+        <v>-5.853658536585</v>
       </c>
       <c r="M18" s="16">
-        <v>42.748091603053</v>
+        <v>39.855072463768</v>
       </c>
       <c r="N18" s="16">
-        <v>-70.08</v>
+        <v>-71.064467766116</v>
       </c>
     </row>
     <row r="19" spans="1:14">
@@ -1031,40 +1031,40 @@
         <v>26</v>
       </c>
       <c r="C19" s="15">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="D19" s="15">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E19" s="16">
-        <v>31.25</v>
+        <v>36.363636363636</v>
       </c>
       <c r="F19" s="15">
-        <v>91</v>
+        <v>117</v>
       </c>
       <c r="G19" s="15">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="H19" s="16">
-        <v>15.189873417721</v>
+        <v>42.682926829268</v>
       </c>
       <c r="I19" s="15">
-        <v>883</v>
+        <v>945</v>
       </c>
       <c r="J19" s="15">
-        <v>550</v>
+        <v>590</v>
       </c>
       <c r="K19" s="16">
-        <v>60.545454545454</v>
+        <v>60.169491525423</v>
       </c>
       <c r="L19" s="16">
-        <v>87.076271186440</v>
+        <v>86.758893280632</v>
       </c>
       <c r="M19" s="16">
-        <v>12.484076433121</v>
+        <v>13.581730769230</v>
       </c>
       <c r="N19" s="16">
-        <v>-69.446366782006</v>
+        <v>-68.996062992126</v>
       </c>
     </row>
     <row r="20" spans="1:14">
@@ -1072,40 +1072,40 @@
         <v>27</v>
       </c>
       <c r="C20" s="15">
-        <v>1</v>
-      </c>
-      <c r="D20" s="15">
-        <v>2</v>
-      </c>
-      <c r="E20" s="16">
-        <v>-50</v>
+        <v>3</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>21</v>
       </c>
       <c r="F20" s="15">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G20" s="15">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H20" s="16">
-        <v>-81.818181818181</v>
+        <v>-53.846153846153</v>
       </c>
       <c r="I20" s="15">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="J20" s="15">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="K20" s="16">
-        <v>11.111111111111</v>
+        <v>3.846153846153</v>
       </c>
       <c r="L20" s="16">
-        <v>92.307692307692</v>
+        <v>107.692307692308</v>
       </c>
       <c r="M20" s="16">
-        <v>56.25</v>
+        <v>68.75</v>
       </c>
       <c r="N20" s="16">
-        <v>-92.559523809523</v>
+        <v>-92.447552447552</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -1113,78 +1113,78 @@
         <v>28</v>
       </c>
       <c r="C21" s="18">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D21" s="18">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="E21" s="19">
-        <v>7.142857142857</v>
+        <v>8.108108108108</v>
       </c>
       <c r="F21" s="18">
-        <v>125</v>
+        <v>151</v>
       </c>
       <c r="G21" s="18">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="H21" s="19">
-        <v>-6.716417910447</v>
+        <v>7.857142857142</v>
       </c>
       <c r="I21" s="18">
-        <v>1336</v>
+        <v>1418</v>
       </c>
       <c r="J21" s="18">
-        <v>890</v>
+        <v>960</v>
       </c>
       <c r="K21" s="19">
-        <v>50.112359550561</v>
+        <v>47.708333333333</v>
       </c>
       <c r="L21" s="19">
-        <v>53.917050691244</v>
+        <v>52.637244348762</v>
       </c>
       <c r="M21" s="19">
-        <v>25.210871602624</v>
+        <v>25.597874224977</v>
       </c>
       <c r="N21" s="19">
-        <v>-73.183460457647</v>
+        <v>-73.031570939520</v>
       </c>
     </row>
     <row r="22" spans="1:14">
       <c r="A22" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="14" t="s">
-        <v>20</v>
+      <c r="C22" s="15">
+        <v>2</v>
       </c>
       <c r="D22" s="15">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E22" s="16">
-        <v>-100</v>
+        <v>-50</v>
       </c>
       <c r="F22" s="15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G22" s="15">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H22" s="16">
-        <v>-72.727272727272</v>
+        <v>-66.666666666666</v>
       </c>
       <c r="I22" s="15">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="J22" s="15">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="K22" s="16">
-        <v>20.689655172413</v>
+        <v>19.354838709677</v>
       </c>
       <c r="L22" s="16">
-        <v>2.941176470588</v>
+        <v>4.225352112676</v>
       </c>
       <c r="M22" s="16">
-        <v>48.936170212766</v>
+        <v>51.020408163265</v>
       </c>
       <c r="N22" s="14" t="s">
         <v>21</v>
@@ -1236,37 +1236,37 @@
         <v>31</v>
       </c>
       <c r="C24" s="15">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D24" s="15">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="E24" s="16">
-        <v>14.285714285714</v>
+        <v>69.565217391304</v>
       </c>
       <c r="F24" s="15">
-        <v>303</v>
+        <v>343</v>
       </c>
       <c r="G24" s="15">
-        <v>228</v>
+        <v>239</v>
       </c>
       <c r="H24" s="16">
-        <v>32.894736842105</v>
+        <v>43.514644351464</v>
       </c>
       <c r="I24" s="15">
-        <v>2896</v>
+        <v>3073</v>
       </c>
       <c r="J24" s="15">
-        <v>1516</v>
+        <v>1621</v>
       </c>
       <c r="K24" s="16">
-        <v>91.029023746701</v>
+        <v>89.574336829117</v>
       </c>
       <c r="L24" s="16">
-        <v>155.154185022026</v>
+        <v>152.713815789474</v>
       </c>
       <c r="M24" s="16">
-        <v>122.256331542594</v>
+        <v>126.288659793814</v>
       </c>
       <c r="N24" s="14" t="s">
         <v>21</v>
@@ -1280,34 +1280,34 @@
         <v>7</v>
       </c>
       <c r="D25" s="15">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E25" s="16">
-        <v>16.666666666666</v>
+        <v>-46.153846153846</v>
       </c>
       <c r="F25" s="15">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="G25" s="15">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="H25" s="16">
-        <v>18.181818181818</v>
+        <v>-28.260869565217</v>
       </c>
       <c r="I25" s="15">
-        <v>274</v>
+        <v>287</v>
       </c>
       <c r="J25" s="15">
-        <v>240</v>
+        <v>266</v>
       </c>
       <c r="K25" s="16">
-        <v>14.166666666666</v>
+        <v>7.894736842105</v>
       </c>
       <c r="L25" s="16">
-        <v>36.318407960199</v>
+        <v>34.741784037558</v>
       </c>
       <c r="M25" s="16">
-        <v>48.108108108108</v>
+        <v>50.261780104712</v>
       </c>
       <c r="N25" s="14" t="s">
         <v>21</v>
@@ -1317,17 +1317,17 @@
       <c r="A26" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="15">
+      <c r="C26" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" s="15">
         <v>2</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F26" s="15">
-        <v>3</v>
       </c>
       <c r="G26" s="14" t="s">
         <v>20</v>
@@ -1345,7 +1345,7 @@
         <v>84.615384615384</v>
       </c>
       <c r="L26" s="16">
-        <v>26.315789473684</v>
+        <v>14.285714285714</v>
       </c>
       <c r="M26" s="14" t="s">
         <v>21</v>
@@ -1359,34 +1359,34 @@
         <v>34</v>
       </c>
       <c r="C27" s="15">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D27" s="15">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E27" s="16">
-        <v>-33.333333333333</v>
+        <v>-14.285714285714</v>
       </c>
       <c r="F27" s="15">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G27" s="15">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H27" s="16">
-        <v>-40</v>
+        <v>-25</v>
       </c>
       <c r="I27" s="15">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="J27" s="15">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="K27" s="16">
-        <v>36.065573770491</v>
+        <v>26.760563380281</v>
       </c>
       <c r="L27" s="16">
-        <v>56.603773584905</v>
+        <v>57.894736842105</v>
       </c>
       <c r="M27" s="14" t="s">
         <v>21</v>
@@ -1430,7 +1430,7 @@
         <v>100</v>
       </c>
       <c r="M28" s="16">
-        <v>-60</v>
+        <v>-66.666666666666</v>
       </c>
       <c r="N28" s="16">
         <v>-50</v>
@@ -1471,7 +1471,7 @@
         <v>100</v>
       </c>
       <c r="M29" s="16">
-        <v>-33.333333333333</v>
+        <v>-50</v>
       </c>
       <c r="N29" s="16">
         <v>-50</v>
@@ -1484,17 +1484,17 @@
       <c r="C30" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D30" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>21</v>
+      <c r="D30" s="15">
+        <v>1</v>
+      </c>
+      <c r="E30" s="16">
+        <v>-100</v>
       </c>
       <c r="F30" s="14" t="s">
         <v>20</v>
       </c>
       <c r="G30" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H30" s="16">
         <v>-100</v>
@@ -1503,13 +1503,13 @@
         <v>10</v>
       </c>
       <c r="J30" s="15">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K30" s="16">
-        <v>11.111111111111</v>
+        <v>0</v>
       </c>
       <c r="L30" s="16">
-        <v>233.333333333333</v>
+        <v>150</v>
       </c>
       <c r="M30" s="14" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
New crime data collected
</commit_message>
<xml_diff>
--- a/data/source/weekly/cs-en-us-001pct.xlsx
+++ b/data/source/weekly/cs-en-us-001pct.xlsx
@@ -69,7 +69,7 @@
         <family val="2"/>
         <rFont val="Andale WT"/>
       </rPr>
-      <t xml:space="preserve">42</t>
+      <t xml:space="preserve">43</t>
     </r>
   </si>
   <si>
@@ -95,7 +95,7 @@
         <family val="2"/>
         <rFont val="Andale WT"/>
       </rPr>
-      <t xml:space="preserve">10/17/2022</t>
+      <t xml:space="preserve">10/24/2022</t>
     </r>
     <r>
       <rPr>
@@ -113,7 +113,7 @@
         <family val="2"/>
         <rFont val="Andale WT"/>
       </rPr>
-      <t xml:space="preserve">10/23/2022</t>
+      <t xml:space="preserve">10/30/2022</t>
     </r>
   </si>
   <si>
@@ -852,8 +852,8 @@
       <c r="K14" s="16">
         <v>-100</v>
       </c>
-      <c r="L14" s="14" t="s">
-        <v>21</v>
+      <c r="L14" s="16">
+        <v>-100</v>
       </c>
       <c r="M14" s="16">
         <v>-100</v>
@@ -866,41 +866,41 @@
       <c r="A15" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="15">
+      <c r="C15" s="15">
         <v>1</v>
       </c>
-      <c r="E15" s="16">
-        <v>-100</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>20</v>
+      <c r="D15" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="15">
+        <v>1</v>
       </c>
       <c r="G15" s="15">
         <v>1</v>
       </c>
       <c r="H15" s="16">
-        <v>-100</v>
+        <v>0</v>
       </c>
       <c r="I15" s="15">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J15" s="15">
         <v>12</v>
       </c>
       <c r="K15" s="16">
-        <v>41.666666666666</v>
+        <v>50</v>
       </c>
       <c r="L15" s="16">
-        <v>-10.526315789473</v>
+        <v>-5.263157894736</v>
       </c>
       <c r="M15" s="16">
-        <v>466.666666666667</v>
+        <v>350</v>
       </c>
       <c r="N15" s="16">
-        <v>54.545454545454</v>
+        <v>63.636363636363</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -908,40 +908,40 @@
         <v>23</v>
       </c>
       <c r="C16" s="15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D16" s="15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E16" s="16">
-        <v>-33.333333333333</v>
+        <v>-25</v>
       </c>
       <c r="F16" s="15">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G16" s="15">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H16" s="16">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I16" s="15">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="J16" s="15">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="K16" s="16">
-        <v>14.583333333333</v>
+        <v>15</v>
       </c>
       <c r="L16" s="16">
-        <v>-9.836065573770</v>
+        <v>-8</v>
       </c>
       <c r="M16" s="16">
-        <v>59.420289855072</v>
+        <v>55.405405405405</v>
       </c>
       <c r="N16" s="16">
-        <v>-84.308131241084</v>
+        <v>-83.848314606741</v>
       </c>
     </row>
     <row r="17" spans="1:14">
@@ -949,13 +949,13 @@
         <v>24</v>
       </c>
       <c r="C17" s="15">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D17" s="15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E17" s="16">
-        <v>500</v>
+        <v>-66.666666666666</v>
       </c>
       <c r="F17" s="15">
         <v>10</v>
@@ -967,22 +967,22 @@
         <v>0</v>
       </c>
       <c r="I17" s="15">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="J17" s="15">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="K17" s="16">
-        <v>14.583333333333</v>
+        <v>12.121212121212</v>
       </c>
       <c r="L17" s="16">
-        <v>61.764705882352</v>
+        <v>54.166666666666</v>
       </c>
       <c r="M17" s="16">
-        <v>96.428571428571</v>
+        <v>94.736842105263</v>
       </c>
       <c r="N17" s="16">
-        <v>-27.152317880794</v>
+        <v>-28.387096774193</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -990,40 +990,40 @@
         <v>25</v>
       </c>
       <c r="C18" s="15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18" s="15">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E18" s="16">
+        <v>-50</v>
+      </c>
+      <c r="F18" s="15">
+        <v>20</v>
+      </c>
+      <c r="G18" s="15">
+        <v>24</v>
+      </c>
+      <c r="H18" s="16">
         <v>-16.666666666666</v>
       </c>
-      <c r="F18" s="15">
-        <v>19</v>
-      </c>
-      <c r="G18" s="15">
-        <v>19</v>
-      </c>
-      <c r="H18" s="16">
-        <v>0</v>
-      </c>
       <c r="I18" s="15">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="J18" s="15">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="K18" s="16">
-        <v>60.465116279069</v>
+        <v>54.014598540146</v>
       </c>
       <c r="L18" s="16">
-        <v>-2.358490566037</v>
+        <v>-1.401869158878</v>
       </c>
       <c r="M18" s="16">
-        <v>41.780821917808</v>
+        <v>43.537414965986</v>
       </c>
       <c r="N18" s="16">
-        <v>-70.470756062767</v>
+        <v>-71.056241426611</v>
       </c>
     </row>
     <row r="19" spans="1:14">
@@ -1031,81 +1031,81 @@
         <v>26</v>
       </c>
       <c r="C19" s="15">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D19" s="15">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E19" s="16">
-        <v>13.043478260869</v>
+        <v>5</v>
       </c>
       <c r="F19" s="15">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="G19" s="15">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H19" s="16">
-        <v>36.046511627907</v>
+        <v>19.318181818181</v>
       </c>
       <c r="I19" s="15">
-        <v>1000</v>
+        <v>1018</v>
       </c>
       <c r="J19" s="15">
-        <v>636</v>
+        <v>656</v>
       </c>
       <c r="K19" s="16">
-        <v>57.232704402515</v>
+        <v>55.182926829268</v>
       </c>
       <c r="L19" s="16">
-        <v>89.035916824196</v>
+        <v>86.788990825688</v>
       </c>
       <c r="M19" s="16">
-        <v>13.250283125707</v>
+        <v>12.362030905077</v>
       </c>
       <c r="N19" s="16">
-        <v>-68.944099378882</v>
+        <v>-69.179533757190</v>
       </c>
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="15">
+      <c r="C20" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="15">
         <v>4</v>
       </c>
-      <c r="D20" s="15">
-        <v>5</v>
-      </c>
       <c r="E20" s="16">
-        <v>-20</v>
+        <v>-100</v>
       </c>
       <c r="F20" s="15">
+        <v>9</v>
+      </c>
+      <c r="G20" s="15">
         <v>10</v>
       </c>
-      <c r="G20" s="15">
-        <v>13</v>
-      </c>
       <c r="H20" s="16">
-        <v>-23.076923076923</v>
+        <v>-10</v>
       </c>
       <c r="I20" s="15">
         <v>60</v>
       </c>
       <c r="J20" s="15">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="K20" s="16">
-        <v>3.448275862068</v>
+        <v>-3.225806451612</v>
       </c>
       <c r="L20" s="16">
         <v>114.285714285714</v>
       </c>
       <c r="M20" s="16">
-        <v>81.818181818181</v>
+        <v>76.470588235294</v>
       </c>
       <c r="N20" s="16">
-        <v>-91.891891891891</v>
+        <v>-92.073976221928</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -1113,40 +1113,40 @@
         <v>28</v>
       </c>
       <c r="C21" s="18">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="D21" s="18">
         <v>39</v>
       </c>
       <c r="E21" s="19">
-        <v>10.256410256410</v>
+        <v>-23.076923076923</v>
       </c>
       <c r="F21" s="18">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="G21" s="18">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="H21" s="19">
-        <v>20.143884892086</v>
+        <v>8.275862068965</v>
       </c>
       <c r="I21" s="18">
-        <v>1504</v>
+        <v>1533</v>
       </c>
       <c r="J21" s="18">
-        <v>1029</v>
+        <v>1068</v>
       </c>
       <c r="K21" s="19">
-        <v>46.161321671525</v>
+        <v>43.539325842696</v>
       </c>
       <c r="L21" s="19">
-        <v>53.783231083844</v>
+        <v>52.689243027888</v>
       </c>
       <c r="M21" s="19">
-        <v>26.174496644295</v>
+        <v>25.245098039215</v>
       </c>
       <c r="N21" s="19">
-        <v>-72.817639616844</v>
+        <v>-72.991543340380</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -1154,37 +1154,37 @@
         <v>29</v>
       </c>
       <c r="C22" s="15">
-        <v>2</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>21</v>
+        <v>3</v>
+      </c>
+      <c r="D22" s="15">
+        <v>1</v>
+      </c>
+      <c r="E22" s="16">
+        <v>200</v>
       </c>
       <c r="F22" s="15">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G22" s="15">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H22" s="16">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="I22" s="15">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="J22" s="15">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K22" s="16">
-        <v>24.193548387096</v>
+        <v>26.984126984127</v>
       </c>
       <c r="L22" s="16">
-        <v>2.666666666666</v>
+        <v>2.564102564102</v>
       </c>
       <c r="M22" s="16">
-        <v>48.076923076923</v>
+        <v>48.148148148148</v>
       </c>
       <c r="N22" s="14" t="s">
         <v>21</v>
@@ -1236,37 +1236,37 @@
         <v>31</v>
       </c>
       <c r="C24" s="15">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D24" s="15">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="E24" s="16">
-        <v>19.402985074626</v>
+        <v>55.102040816326</v>
       </c>
       <c r="F24" s="15">
-        <v>325</v>
+        <v>302</v>
       </c>
       <c r="G24" s="15">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="H24" s="16">
-        <v>40.086206896551</v>
+        <v>36.036036036036</v>
       </c>
       <c r="I24" s="15">
-        <v>3221</v>
+        <v>3297</v>
       </c>
       <c r="J24" s="15">
-        <v>1748</v>
+        <v>1797</v>
       </c>
       <c r="K24" s="16">
-        <v>84.267734553775</v>
+        <v>83.472454090150</v>
       </c>
       <c r="L24" s="16">
-        <v>140.732436472347</v>
+        <v>138.222543352601</v>
       </c>
       <c r="M24" s="16">
-        <v>128.601845280341</v>
+        <v>130.720783764871</v>
       </c>
       <c r="N24" s="14" t="s">
         <v>21</v>
@@ -1277,37 +1277,37 @@
         <v>32</v>
       </c>
       <c r="C25" s="15">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D25" s="15">
         <v>11</v>
       </c>
       <c r="E25" s="16">
-        <v>0</v>
+        <v>-54.545454545454</v>
       </c>
       <c r="F25" s="15">
         <v>32</v>
       </c>
       <c r="G25" s="15">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H25" s="16">
-        <v>-27.272727272727</v>
+        <v>-23.809523809523</v>
       </c>
       <c r="I25" s="15">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="J25" s="15">
-        <v>284</v>
+        <v>295</v>
       </c>
       <c r="K25" s="16">
-        <v>7.746478873239</v>
+        <v>5.762711864406</v>
       </c>
       <c r="L25" s="16">
-        <v>37.837837837837</v>
+        <v>37.444933920704</v>
       </c>
       <c r="M25" s="16">
-        <v>51.485148514851</v>
+        <v>49.282296650717</v>
       </c>
       <c r="N25" s="14" t="s">
         <v>21</v>
@@ -1317,35 +1317,35 @@
       <c r="A26" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D26" s="15">
+      <c r="C26" s="15">
         <v>1</v>
       </c>
-      <c r="E26" s="16">
-        <v>-100</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>20</v>
+      <c r="D26" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" s="15">
+        <v>1</v>
       </c>
       <c r="G26" s="15">
         <v>1</v>
       </c>
       <c r="H26" s="16">
-        <v>-100</v>
+        <v>0</v>
       </c>
       <c r="I26" s="15">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J26" s="15">
         <v>14</v>
       </c>
       <c r="K26" s="16">
-        <v>71.428571428571</v>
+        <v>78.571428571428</v>
       </c>
       <c r="L26" s="16">
-        <v>9.090909090909</v>
+        <v>13.636363636363</v>
       </c>
       <c r="M26" s="14" t="s">
         <v>21</v>
@@ -1358,32 +1358,32 @@
       <c r="A27" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="15">
-        <v>3</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E27" s="14" t="s">
-        <v>21</v>
+      <c r="C27" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" s="15">
+        <v>1</v>
+      </c>
+      <c r="E27" s="16">
+        <v>-100</v>
       </c>
       <c r="F27" s="15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G27" s="15">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H27" s="16">
-        <v>27.272727272727</v>
+        <v>44.444444444444</v>
       </c>
       <c r="I27" s="15">
         <v>97</v>
       </c>
       <c r="J27" s="15">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K27" s="16">
-        <v>34.722222222222</v>
+        <v>32.876712328767</v>
       </c>
       <c r="L27" s="16">
         <v>61.666666666666</v>
@@ -1427,7 +1427,7 @@
         <v>21</v>
       </c>
       <c r="L28" s="16">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="M28" s="16">
         <v>-66.666666666666</v>
@@ -1468,7 +1468,7 @@
         <v>21</v>
       </c>
       <c r="L29" s="16">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="M29" s="16">
         <v>-50</v>

</xml_diff>